<commit_message>
delete unused yml files
</commit_message>
<xml_diff>
--- a/createdRecords.xlsx
+++ b/createdRecords.xlsx
@@ -422,7 +422,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A48"/>
+  <dimension ref="A1:A51"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -667,17 +667,32 @@
         <v>A227258</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>A227305</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>A227306</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>A227307</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A48"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A51"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A26"/>
+  <dimension ref="A1:A27"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -752,17 +767,22 @@
         <v>P-860360</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>P-860402</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A26"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A27"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A35"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -942,10 +962,25 @@
         <v>R02162</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>R02176</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>R02178</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>R02180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A35"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A38"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>